<commit_message>
made changes to axis_with_login.py for detecting error webpages
</commit_message>
<xml_diff>
--- a/link_check_report.xlsx
+++ b/link_check_report.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://www.rbi.org.in</t>
+          <t>https://www.google.com</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -466,7 +466,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://www.owasp.org</t>
+          <t>https://www.sebi.gov.in</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -486,7 +486,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://www.sebi.gov.in</t>
+          <t>https://www.surveymonkey.com</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://www.axisbank.com</t>
+          <t>https://www.owasp.org</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -526,7 +526,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://www.surveymonkey.com</t>
+          <t>https://www.axisbank.com</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -546,18 +546,35 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://www.google.com</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
+          <t>https://www.sahilendworldfibvweuidbuk.org</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Not Checked</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>HTTPSConnectionPool(host='www.sahilendworldfibvweuidbuk.org', port=443): Max retries exceeded with url: / (Caused by NameResolutionError("&lt;urllib3.connection.HTTPSConnection object at 0x000001CC7FEB4550&gt;: Failed to resolve 'www.sahilendworldfibvweuidbuk.org' ([Errno 11001] getaddrinfo failed)"))</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>https://www.rbi.org.in</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
         <v>200</v>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>Checked</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>Success</t>
         </is>

</xml_diff>

<commit_message>
Revert project to commit f4eed51
</commit_message>
<xml_diff>
--- a/link_check_report.xlsx
+++ b/link_check_report.xlsx
@@ -446,24 +446,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://www.sahilendworldfibvweuidbuk.org</t>
-        </is>
+          <t>https://www.google.com</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>200</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Not Checked</t>
+          <t>Checked</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>HTTPSConnectionPool(host='www.sahilendworldfibvweuidbuk.org', port=443): Max retries exceeded with url: / (Caused by NameResolutionError("&lt;urllib3.connection.HTTPSConnection object at 0x0000023974E75090&gt;: Failed to resolve 'www.sahilendworldfibvweuidbuk.org' ([Errno 11001] getaddrinfo failed)"))</t>
+          <t>Success</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://www.axisbank.com</t>
+          <t>https://www.sebi.gov.in</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -503,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://www.rbi.org.in</t>
+          <t>https://www.owasp.org</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -523,7 +526,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://www.sebi.gov.in</t>
+          <t>https://www.axisbank.com</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -543,27 +546,24 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://www.owasp.org</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>200</v>
+          <t>https://www.sahilendworldfibvweuidbuk.org</t>
+        </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Checked</t>
+          <t>Not Checked</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Success</t>
+          <t>HTTPSConnectionPool(host='www.sahilendworldfibvweuidbuk.org', port=443): Max retries exceeded with url: / (Caused by NameResolutionError("&lt;urllib3.connection.HTTPSConnection object at 0x000001CC7FEB4550&gt;: Failed to resolve 'www.sahilendworldfibvweuidbuk.org' ([Errno 11001] getaddrinfo failed)"))</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>https://www.google.com</t>
+          <t>https://www.rbi.org.in</t>
         </is>
       </c>
       <c r="B8" t="n">

</xml_diff>